<commit_message>
Fixed sprint and performance tables
</commit_message>
<xml_diff>
--- a/input_data/team_code_orbit_data.xlsx
+++ b/input_data/team_code_orbit_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyedAtyabHussain\Documents\work_area\PerformanceReportGenerator\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC5AF9D-E54F-49EC-931E-2DCA51644A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8681311F-06D7-45E8-B09B-C78CF983AD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{6157CC41-DCF7-4F8D-AFDE-C223C9483824}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="424">
   <si>
     <t>Name</t>
   </si>
@@ -1165,9 +1165,6 @@
   </si>
   <si>
     <t>Sprint commitments vs deliveries total score (out of 10%)</t>
-  </si>
-  <si>
-    <t>Tecnical Interview (out of 90%)</t>
   </si>
   <si>
     <t>Comments</t>
@@ -2127,9 +2124,9 @@
     <tableColumn id="12" xr3:uid="{D6BCF59B-0D54-4281-BDAD-1CB545376E44}" name="Decision Making"/>
     <tableColumn id="13" xr3:uid="{B05021CB-F518-4A3A-89B3-3E52E5FF2274}" name="Punctuality"/>
     <tableColumn id="14" xr3:uid="{7695CCAD-0913-4210-9418-99465480AA62}" name="Sprint commitments vs deliveries total score (out of 10%)"/>
-    <tableColumn id="15" xr3:uid="{3DF9F017-2960-4559-ACB1-F3D258EBB795}" name="Tecnical Interview (out of 90%)" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{3DF9F017-2960-4559-ACB1-F3D258EBB795}" name="Final Evaluation (out of 90%)" dataDxfId="1"/>
     <tableColumn id="17" xr3:uid="{BF21469E-331F-4FEE-8F48-9FF26DD1C857}" name="Total Score (out of 100%)" dataDxfId="0">
-      <calculatedColumnFormula>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{AC0CCED6-3179-4D61-A3C7-B75FA9970889}" name="Comments"/>
   </tableColumns>
@@ -3763,7 +3760,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -5181,7 +5178,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -6599,7 +6596,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -8017,7 +8014,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -9363,7 +9360,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -9478,9 +9475,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289C827E-09D4-481A-A67E-0EFC3E492384}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9547,13 +9544,13 @@
         <v>347</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -9603,11 +9600,11 @@
         <v>1.08</v>
       </c>
       <c r="P2" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>1.08</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -9657,11 +9654,11 @@
         <v>0.63</v>
       </c>
       <c r="P3" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.73</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -9711,11 +9708,11 @@
         <v>0.27</v>
       </c>
       <c r="P4" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.27</v>
       </c>
       <c r="Q4" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -9765,11 +9762,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="P5" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -9817,7 +9814,7 @@
       </c>
       <c r="O6" s="25"/>
       <c r="P6" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0</v>
       </c>
       <c r="Q6" s="21"/>
@@ -9869,7 +9866,7 @@
         <v>0.27</v>
       </c>
       <c r="P7" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.37</v>
       </c>
       <c r="Q7" s="21"/>
@@ -9921,7 +9918,7 @@
         <v>0.54</v>
       </c>
       <c r="P8" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.64</v>
       </c>
       <c r="Q8" s="21"/>
@@ -9973,11 +9970,11 @@
         <v>0.63</v>
       </c>
       <c r="P9" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.73</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -10027,11 +10024,11 @@
         <v>0.81</v>
       </c>
       <c r="P10" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.81</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -10081,7 +10078,7 @@
         <v>0.27</v>
       </c>
       <c r="P11" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.27</v>
       </c>
       <c r="Q11" s="21"/>
@@ -10133,7 +10130,7 @@
         <v>0.27</v>
       </c>
       <c r="P12" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.27</v>
       </c>
       <c r="Q12" s="21"/>
@@ -10185,11 +10182,11 @@
         <v>1.08</v>
       </c>
       <c r="P13" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>1.1800000000000002</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10239,11 +10236,11 @@
         <v>0.09</v>
       </c>
       <c r="P14" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.09</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -10293,7 +10290,7 @@
         <v>0.36</v>
       </c>
       <c r="P15" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.36</v>
       </c>
       <c r="Q15" s="21"/>
@@ -10345,7 +10342,7 @@
         <v>0.45</v>
       </c>
       <c r="P16" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="Q16" s="21"/>
@@ -10397,11 +10394,11 @@
         <v>0.54</v>
       </c>
       <c r="P17" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.54</v>
       </c>
       <c r="Q17" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10451,11 +10448,11 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="P18" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.13500000000000001</v>
       </c>
       <c r="Q18" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10505,11 +10502,11 @@
         <v>1.17</v>
       </c>
       <c r="P19" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>1.27</v>
       </c>
       <c r="Q19" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -10559,7 +10556,7 @@
         <v>0.54</v>
       </c>
       <c r="P20" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.54</v>
       </c>
       <c r="Q20" s="21"/>
@@ -10611,11 +10608,11 @@
         <v>2.7E-2</v>
       </c>
       <c r="P21" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>2.7E-2</v>
       </c>
       <c r="Q21" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10665,11 +10662,11 @@
         <v>0.89100000000000001</v>
       </c>
       <c r="P22" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.89100000000000001</v>
       </c>
       <c r="Q22" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10719,11 +10716,11 @@
         <v>0.72</v>
       </c>
       <c r="P23" s="27">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0.82</v>
       </c>
       <c r="Q23" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -10743,7 +10740,7 @@
       <c r="N24" s="4"/>
       <c r="O24" s="8"/>
       <c r="P24" s="4">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0</v>
       </c>
     </row>
@@ -10764,13 +10761,13 @@
       <c r="N25" s="4"/>
       <c r="O25" s="8"/>
       <c r="P25" s="4">
-        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Tecnical Interview (out of 90%)]])</f>
+        <f>SUM(Table1[[#This Row],[Sprint commitments vs deliveries total score (out of 10%)]:[Final Evaluation (out of 90%)]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -10782,26 +10779,26 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>364</v>
-      </c>
-      <c r="C27" t="s">
-        <v>365</v>
       </c>
       <c r="O27" s="19"/>
       <c r="P27"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>367</v>
-      </c>
-      <c r="C28" t="s">
-        <v>368</v>
       </c>
       <c r="O28" s="19"/>
       <c r="P28"/>
@@ -10892,7 +10889,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O21" sqref="O21"/>
+      <selection pane="topRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10958,7 +10955,7 @@
         <v>347</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>16</v>
@@ -12122,7 +12119,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -12137,24 +12134,24 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>371</v>
-      </c>
-      <c r="C27" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>374</v>
-      </c>
-      <c r="C28" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -12256,27 +12253,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1" t="s">
         <v>376</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>377</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>378</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>379</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>380</v>
-      </c>
-      <c r="F1" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2">
         <v>68</v>
@@ -12288,7 +12285,7 @@
         <v>307</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F2" s="15">
         <v>1</v>
@@ -12296,7 +12293,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B3">
         <v>61.5</v>
@@ -12316,7 +12313,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B4">
         <v>69.600000000000009</v>
@@ -12328,7 +12325,7 @@
         <v>307</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F4" s="15">
         <v>1</v>
@@ -12336,7 +12333,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B5">
         <v>74</v>
@@ -12348,7 +12345,7 @@
         <v>307</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F5" s="15">
         <v>1</v>
@@ -12356,7 +12353,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B6">
         <v>69.899999999999991</v>
@@ -12368,7 +12365,7 @@
         <v>307</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
@@ -12376,7 +12373,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B7">
         <v>67.400000000000006</v>
@@ -12388,7 +12385,7 @@
         <v>307</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F7" s="15">
         <v>1</v>
@@ -12396,7 +12393,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B8">
         <v>62.9</v>
@@ -12408,7 +12405,7 @@
         <v>307</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F8" s="15">
         <v>1</v>
@@ -12416,7 +12413,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B9">
         <v>63.2</v>
@@ -12428,7 +12425,7 @@
         <v>307</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F9" s="15">
         <v>1</v>
@@ -12436,7 +12433,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B10">
         <v>63.8</v>
@@ -12448,7 +12445,7 @@
         <v>307</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F10" s="15">
         <v>1</v>
@@ -12456,7 +12453,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B11">
         <v>62.5</v>
@@ -12468,7 +12465,7 @@
         <v>307</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F11" s="15">
         <v>1</v>
@@ -12476,7 +12473,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B12">
         <v>67.599999999999994</v>
@@ -12488,7 +12485,7 @@
         <v>307</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F12" s="15">
         <v>1</v>
@@ -12496,7 +12493,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B13">
         <v>63.599999999999994</v>
@@ -12508,7 +12505,7 @@
         <v>307</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F13" s="15">
         <v>1</v>
@@ -12516,7 +12513,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B14">
         <v>77.099999999999994</v>
@@ -12528,7 +12525,7 @@
         <v>307</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F14" s="15">
         <v>1</v>
@@ -12548,7 +12545,7 @@
         <v>307</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F15" s="15">
         <v>1</v>
@@ -12556,7 +12553,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B16">
         <v>70.599999999999994</v>
@@ -12568,7 +12565,7 @@
         <v>307</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F16" s="15">
         <v>1</v>
@@ -12576,7 +12573,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B17">
         <v>56.8</v>
@@ -12588,7 +12585,7 @@
         <v>307</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F17" s="15">
         <v>1</v>
@@ -12596,7 +12593,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B18">
         <v>63.4</v>
@@ -12608,7 +12605,7 @@
         <v>307</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F18" s="15">
         <v>1</v>
@@ -12616,7 +12613,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B19">
         <v>65.2</v>
@@ -12628,7 +12625,7 @@
         <v>307</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F19" s="15">
         <v>1</v>
@@ -12636,7 +12633,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B20">
         <v>64</v>
@@ -12648,7 +12645,7 @@
         <v>307</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F20" s="15">
         <v>1</v>
@@ -12656,7 +12653,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B21">
         <v>50.1</v>
@@ -12668,7 +12665,7 @@
         <v>307</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F21" s="15">
         <v>1</v>
@@ -12676,7 +12673,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B22">
         <v>51.7</v>
@@ -12688,7 +12685,7 @@
         <v>307</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
@@ -12696,7 +12693,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B23" s="11">
         <v>42.9</v>
@@ -12708,7 +12705,7 @@
         <v>307</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F23" s="15">
         <v>1</v>
@@ -12964,6 +12961,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="5524ecfe-089c-425a-a4be-7743da73ddfc" xsi:nil="true"/>
@@ -12972,15 +12978,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13003,6 +13000,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A92F8EAB-94F8-4973-85AA-EF84B5AC7367}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3006C25A-5E3C-49E7-B071-5EAE6BA5B6FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -13011,12 +13016,4 @@
     <ds:schemaRef ds:uri="7112d4b0-5493-499c-a8a1-c4cefa8f8360"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A92F8EAB-94F8-4973-85AA-EF84B5AC7367}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corrected input data and refactored conditional statements
</commit_message>
<xml_diff>
--- a/input_data/team_code_orbit_data.xlsx
+++ b/input_data/team_code_orbit_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyedAtyabHussain\Documents\work_area\PerformanceReportGenerator\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8681311F-06D7-45E8-B09B-C78CF983AD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92243D5-DAC6-4C26-A5FA-2305013C1060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{6157CC41-DCF7-4F8D-AFDE-C223C9483824}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6157CC41-DCF7-4F8D-AFDE-C223C9483824}"/>
   </bookViews>
   <sheets>
     <sheet name="April 2025" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2303" uniqueCount="423">
   <si>
     <t>Name</t>
   </si>
@@ -1093,9 +1093,6 @@
   </si>
   <si>
     <t>Web APIs</t>
-  </si>
-  <si>
-    <t>Mini Quizzes total score (out of 00%)</t>
   </si>
   <si>
     <t>Monthly Evaluation (out of 50%)</t>
@@ -3760,7 +3757,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -5178,7 +5175,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -5288,11 +5285,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E8CBCC-0E08-436D-8B3C-C0F491552F1B}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5310,12 +5307,11 @@
     <col min="12" max="12" width="61.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="62.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5358,17 +5354,14 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -5411,18 +5404,15 @@
       <c r="N2">
         <v>50</v>
       </c>
-      <c r="O2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="6">
-        <v>38.729999999999997</v>
-      </c>
-      <c r="Q2">
-        <f t="shared" ref="Q2:Q23" si="0">SUM(N2,O2,P2)</f>
-        <v>88.72999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O2" s="6">
+        <v>48.41</v>
+      </c>
+      <c r="P2">
+        <f>SUM(N2,O2)</f>
+        <v>98.41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -5465,18 +5455,15 @@
       <c r="N3">
         <v>50</v>
       </c>
-      <c r="O3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="6">
-        <v>36.96</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" si="0"/>
-        <v>86.960000000000008</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O3" s="6">
+        <v>46.2</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P23" si="0">SUM(N3,O3)</f>
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
@@ -5502,7 +5489,7 @@
         <v>311</v>
       </c>
       <c r="I4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>312</v>
@@ -5519,18 +5506,15 @@
       <c r="N4">
         <v>20</v>
       </c>
-      <c r="O4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P4" s="6">
+      <c r="O4" s="6">
         <v>0</v>
       </c>
-      <c r="Q4">
+      <c r="P4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -5573,18 +5557,15 @@
       <c r="N5">
         <v>50</v>
       </c>
-      <c r="O5" t="s">
-        <v>46</v>
-      </c>
-      <c r="P5" s="6">
-        <v>31.9</v>
-      </c>
-      <c r="Q5">
+      <c r="O5" s="6">
+        <v>39.880000000000003</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="0"/>
-        <v>81.900000000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>89.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -5627,18 +5608,15 @@
       <c r="N6">
         <v>50</v>
       </c>
-      <c r="O6" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" s="6">
-        <v>27.85</v>
-      </c>
-      <c r="Q6">
+      <c r="O6" s="6">
+        <v>34.81</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="0"/>
-        <v>77.849999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>84.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
@@ -5681,18 +5659,15 @@
       <c r="N7">
         <v>40</v>
       </c>
-      <c r="O7" t="s">
-        <v>46</v>
-      </c>
-      <c r="P7" s="6">
-        <v>30.89</v>
-      </c>
-      <c r="Q7">
+      <c r="O7" s="6">
+        <v>38.61</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="0"/>
-        <v>70.89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>78.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>95</v>
       </c>
@@ -5735,18 +5710,15 @@
       <c r="N8">
         <v>50</v>
       </c>
-      <c r="O8" t="s">
-        <v>46</v>
-      </c>
-      <c r="P8" s="6">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="Q8">
+      <c r="O8" s="6">
+        <v>45.25</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="0"/>
-        <v>86.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>95.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>108</v>
       </c>
@@ -5789,18 +5761,15 @@
       <c r="N9">
         <v>50</v>
       </c>
-      <c r="O9" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" s="6">
-        <v>31.65</v>
-      </c>
-      <c r="Q9">
+      <c r="O9" s="6">
+        <v>39.56</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="0"/>
-        <v>81.650000000000006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>89.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -5843,18 +5812,15 @@
       <c r="N10">
         <v>40</v>
       </c>
-      <c r="O10" t="s">
-        <v>46</v>
-      </c>
-      <c r="P10" s="6">
-        <v>34.68</v>
-      </c>
-      <c r="Q10">
+      <c r="O10" s="6">
+        <v>43.35</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="0"/>
-        <v>74.680000000000007</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>83.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>134</v>
       </c>
@@ -5897,18 +5863,15 @@
       <c r="N11">
         <v>40</v>
       </c>
-      <c r="O11" t="s">
-        <v>46</v>
-      </c>
-      <c r="P11" s="6">
-        <v>25.82</v>
-      </c>
-      <c r="Q11">
+      <c r="O11" s="6">
+        <v>32.28</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="0"/>
-        <v>65.819999999999993</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>72.28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>147</v>
       </c>
@@ -5951,18 +5914,15 @@
       <c r="N12">
         <v>40</v>
       </c>
-      <c r="O12" t="s">
-        <v>46</v>
-      </c>
-      <c r="P12" s="6">
-        <v>35.44</v>
-      </c>
-      <c r="Q12">
+      <c r="O12" s="6">
+        <v>44.3</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="0"/>
-        <v>75.44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>160</v>
       </c>
@@ -6005,18 +5965,15 @@
       <c r="N13">
         <v>50</v>
       </c>
-      <c r="O13" t="s">
-        <v>46</v>
-      </c>
-      <c r="P13" s="6">
-        <v>39.24</v>
-      </c>
-      <c r="Q13">
+      <c r="O13" s="6">
+        <v>49.05</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="0"/>
-        <v>89.240000000000009</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>99.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>173</v>
       </c>
@@ -6059,18 +6016,15 @@
       <c r="N14">
         <v>50</v>
       </c>
-      <c r="O14" t="s">
-        <v>46</v>
-      </c>
-      <c r="P14" s="6">
-        <v>25.25</v>
-      </c>
-      <c r="Q14">
+      <c r="O14" s="6">
+        <v>31.56</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="0"/>
-        <v>75.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>81.56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>186</v>
       </c>
@@ -6113,18 +6067,15 @@
       <c r="N15">
         <v>45</v>
       </c>
-      <c r="O15" t="s">
-        <v>46</v>
-      </c>
-      <c r="P15" s="6">
-        <v>30.89</v>
-      </c>
-      <c r="Q15">
+      <c r="O15" s="6">
+        <v>38.61</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="0"/>
-        <v>75.89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>83.61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>199</v>
       </c>
@@ -6167,18 +6118,15 @@
       <c r="N16">
         <v>50</v>
       </c>
-      <c r="O16" t="s">
-        <v>46</v>
-      </c>
-      <c r="P16" s="6">
-        <v>32.659999999999997</v>
-      </c>
-      <c r="Q16">
+      <c r="O16" s="6">
+        <v>40.83</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="0"/>
-        <v>82.66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>90.83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>212</v>
       </c>
@@ -6221,18 +6169,15 @@
       <c r="N17">
         <v>50</v>
       </c>
-      <c r="O17" t="s">
-        <v>46</v>
-      </c>
-      <c r="P17" s="6">
-        <v>37.72</v>
-      </c>
-      <c r="Q17">
+      <c r="O17" s="6">
+        <v>47.15</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="0"/>
-        <v>87.72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>97.15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>224</v>
       </c>
@@ -6275,18 +6220,15 @@
       <c r="N18">
         <v>50</v>
       </c>
-      <c r="O18" t="s">
-        <v>46</v>
-      </c>
-      <c r="P18" s="6">
-        <v>20.25</v>
-      </c>
-      <c r="Q18">
+      <c r="O18" s="6">
+        <v>25.31</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="0"/>
-        <v>70.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>75.31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>236</v>
       </c>
@@ -6329,18 +6271,15 @@
       <c r="N19">
         <v>50</v>
       </c>
-      <c r="O19" t="s">
-        <v>46</v>
-      </c>
-      <c r="P19" s="6">
-        <v>36.46</v>
-      </c>
-      <c r="Q19">
+      <c r="O19" s="6">
+        <v>45.58</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="0"/>
-        <v>86.460000000000008</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <v>95.58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>249</v>
       </c>
@@ -6383,18 +6322,15 @@
       <c r="N20">
         <v>50</v>
       </c>
-      <c r="O20" t="s">
-        <v>46</v>
-      </c>
-      <c r="P20" s="6">
-        <v>33.92</v>
-      </c>
-      <c r="Q20">
+      <c r="O20" s="6">
+        <v>42.4</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="0"/>
-        <v>83.92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>262</v>
       </c>
@@ -6437,18 +6373,15 @@
       <c r="N21">
         <v>40</v>
       </c>
-      <c r="O21" t="s">
-        <v>46</v>
-      </c>
-      <c r="P21" s="6">
-        <v>31.14</v>
-      </c>
-      <c r="Q21">
+      <c r="O21" s="6">
+        <v>38.93</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="0"/>
-        <v>71.14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>78.930000000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>273</v>
       </c>
@@ -6491,18 +6424,15 @@
       <c r="N22">
         <v>50</v>
       </c>
-      <c r="O22" t="s">
-        <v>46</v>
-      </c>
-      <c r="P22" s="6">
-        <v>35</v>
-      </c>
-      <c r="Q22">
+      <c r="O22" s="6">
+        <v>43.75</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>285</v>
       </c>
@@ -6545,18 +6475,15 @@
       <c r="N23">
         <v>50</v>
       </c>
-      <c r="O23" t="s">
-        <v>46</v>
-      </c>
-      <c r="P23" s="6">
-        <v>30</v>
-      </c>
-      <c r="Q23">
+      <c r="O23" s="6">
+        <v>37.5</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -6571,11 +6498,10 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O24" s="8"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -6590,13 +6516,12 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="4"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O25" s="8"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -6605,29 +6530,29 @@
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>328</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>331</v>
       </c>
-      <c r="C28" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -6642,11 +6567,10 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="4"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O29" s="8"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -6661,11 +6585,10 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="4"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O30" s="8"/>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>306</v>
       </c>
@@ -6673,7 +6596,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
         <v>308</v>
       </c>
@@ -6709,7 +6632,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -8014,7 +7937,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -8025,24 +7948,24 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>334</v>
-      </c>
-      <c r="C27" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>337</v>
-      </c>
-      <c r="C28" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -8126,8 +8049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CBED5A-119B-4DD0-A3C0-DD4B7D4EF36A}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -8194,7 +8117,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>16</v>
@@ -9360,7 +9283,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -9371,24 +9294,24 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>341</v>
-      </c>
-      <c r="C27" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>344</v>
-      </c>
-      <c r="C28" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -9453,7 +9376,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -9541,16 +9464,16 @@
         <v>12</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -9604,7 +9527,7 @@
         <v>1.08</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -9658,7 +9581,7 @@
         <v>0.73</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -9712,7 +9635,7 @@
         <v>0.27</v>
       </c>
       <c r="Q4" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -9766,7 +9689,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -9974,7 +9897,7 @@
         <v>0.73</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -10028,7 +9951,7 @@
         <v>0.81</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -10186,7 +10109,7 @@
         <v>1.1800000000000002</v>
       </c>
       <c r="Q13" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10240,7 +10163,7 @@
         <v>0.09</v>
       </c>
       <c r="Q14" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -10398,7 +10321,7 @@
         <v>0.54</v>
       </c>
       <c r="Q17" s="21" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10452,7 +10375,7 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="Q18" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10506,7 +10429,7 @@
         <v>1.27</v>
       </c>
       <c r="Q19" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -10612,7 +10535,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="Q21" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10666,7 +10589,7 @@
         <v>0.89100000000000001</v>
       </c>
       <c r="Q22" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -10720,7 +10643,7 @@
         <v>0.82</v>
       </c>
       <c r="Q23" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -10767,7 +10690,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -10779,26 +10702,26 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>363</v>
-      </c>
-      <c r="C27" t="s">
-        <v>364</v>
       </c>
       <c r="O27" s="19"/>
       <c r="P27"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>366</v>
-      </c>
-      <c r="C28" t="s">
-        <v>367</v>
       </c>
       <c r="O28" s="19"/>
       <c r="P28"/>
@@ -10887,7 +10810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FFF526-E116-4DC6-8235-CFE7596CA50F}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
     </sheetView>
@@ -10952,10 +10875,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>16</v>
@@ -12119,7 +12042,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>298</v>
@@ -12134,24 +12057,24 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>370</v>
-      </c>
-      <c r="C27" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>373</v>
-      </c>
-      <c r="C28" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -12253,27 +12176,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" t="s">
         <v>375</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>376</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>377</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>378</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>379</v>
-      </c>
-      <c r="F1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B2">
         <v>68</v>
@@ -12285,7 +12208,7 @@
         <v>307</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F2" s="15">
         <v>1</v>
@@ -12293,7 +12216,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B3">
         <v>61.5</v>
@@ -12313,7 +12236,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B4">
         <v>69.600000000000009</v>
@@ -12325,7 +12248,7 @@
         <v>307</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F4" s="15">
         <v>1</v>
@@ -12333,7 +12256,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B5">
         <v>74</v>
@@ -12345,7 +12268,7 @@
         <v>307</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F5" s="15">
         <v>1</v>
@@ -12353,7 +12276,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B6">
         <v>69.899999999999991</v>
@@ -12365,7 +12288,7 @@
         <v>307</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
@@ -12373,7 +12296,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B7">
         <v>67.400000000000006</v>
@@ -12385,7 +12308,7 @@
         <v>307</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F7" s="15">
         <v>1</v>
@@ -12393,7 +12316,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B8">
         <v>62.9</v>
@@ -12405,7 +12328,7 @@
         <v>307</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F8" s="15">
         <v>1</v>
@@ -12413,7 +12336,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B9">
         <v>63.2</v>
@@ -12425,7 +12348,7 @@
         <v>307</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F9" s="15">
         <v>1</v>
@@ -12433,7 +12356,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B10">
         <v>63.8</v>
@@ -12445,7 +12368,7 @@
         <v>307</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F10" s="15">
         <v>1</v>
@@ -12453,7 +12376,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B11">
         <v>62.5</v>
@@ -12465,7 +12388,7 @@
         <v>307</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F11" s="15">
         <v>1</v>
@@ -12473,7 +12396,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B12">
         <v>67.599999999999994</v>
@@ -12485,7 +12408,7 @@
         <v>307</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F12" s="15">
         <v>1</v>
@@ -12493,7 +12416,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B13">
         <v>63.599999999999994</v>
@@ -12505,7 +12428,7 @@
         <v>307</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F13" s="15">
         <v>1</v>
@@ -12513,7 +12436,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B14">
         <v>77.099999999999994</v>
@@ -12525,7 +12448,7 @@
         <v>307</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F14" s="15">
         <v>1</v>
@@ -12545,7 +12468,7 @@
         <v>307</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F15" s="15">
         <v>1</v>
@@ -12553,7 +12476,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B16">
         <v>70.599999999999994</v>
@@ -12565,7 +12488,7 @@
         <v>307</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F16" s="15">
         <v>1</v>
@@ -12573,7 +12496,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B17">
         <v>56.8</v>
@@ -12585,7 +12508,7 @@
         <v>307</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F17" s="15">
         <v>1</v>
@@ -12593,7 +12516,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B18">
         <v>63.4</v>
@@ -12605,7 +12528,7 @@
         <v>307</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F18" s="15">
         <v>1</v>
@@ -12613,7 +12536,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B19">
         <v>65.2</v>
@@ -12625,7 +12548,7 @@
         <v>307</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F19" s="15">
         <v>1</v>
@@ -12633,7 +12556,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B20">
         <v>64</v>
@@ -12645,7 +12568,7 @@
         <v>307</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F20" s="15">
         <v>1</v>
@@ -12653,7 +12576,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B21">
         <v>50.1</v>
@@ -12665,7 +12588,7 @@
         <v>307</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F21" s="15">
         <v>1</v>
@@ -12673,7 +12596,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B22">
         <v>51.7</v>
@@ -12685,7 +12608,7 @@
         <v>307</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F22" s="15">
         <v>1</v>
@@ -12693,7 +12616,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B23" s="11">
         <v>42.9</v>
@@ -12705,7 +12628,7 @@
         <v>307</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F23" s="15">
         <v>1</v>
@@ -12961,15 +12884,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="5524ecfe-089c-425a-a4be-7743da73ddfc" xsi:nil="true"/>
@@ -12978,6 +12892,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13000,14 +12923,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A92F8EAB-94F8-4973-85AA-EF84B5AC7367}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3006C25A-5E3C-49E7-B071-5EAE6BA5B6FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -13016,4 +12931,12 @@
     <ds:schemaRef ds:uri="7112d4b0-5493-499c-a8a1-c4cefa8f8360"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A92F8EAB-94F8-4973-85AA-EF84B5AC7367}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>